<commit_message>
Added AppendMetadataToExcel.xaml and AddToQueue.xaml workflows for Excel update and queue integration
</commit_message>
<xml_diff>
--- a/Data/Output/PartnershipEmails_Report.xlsx
+++ b/Data/Output/PartnershipEmails_Report.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Desktop\T2G_EmailAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBD5D52-ADEB-4160-B468-ACE7938A1775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BF24DD-A887-4BEA-97D7-2185F6644BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Partnership_Emails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date Processed</t>
   </si>
@@ -46,6 +46,26 @@
   </si>
   <si>
     <t>Email Subject</t>
+  </si>
+  <si>
+    <t>Moris Mwai</t>
+  </si>
+  <si>
+    <t>Tech-Neo GmbH</t>
+  </si>
+  <si>
+    <t>Am main City, Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE1567890_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>morismwai1@gmail.com</t>
+  </si>
+  <si>
+    <t>Partnership Offer</t>
   </si>
 </sst>
 </file>
@@ -89,9 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,17 +396,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -408,6 +436,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45854.104351851849</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Process.xaml to handle email and queue population
</commit_message>
<xml_diff>
--- a/Data/Output/PartnershipEmails_Report.xlsx
+++ b/Data/Output/PartnershipEmails_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{65BF24DD-A887-4BEA-97D7-2185F6644BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E05D195B-C752-4F8C-BDF1-9573CDB4BC2F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{65BF24DD-A887-4BEA-97D7-2185F6644BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{528C62C7-AC8D-4C6D-84D5-15998BE8A9BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partnership_Emails" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
   <si>
     <t>Date Processed</t>
   </si>
@@ -133,6 +133,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -691,6 +695,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45854.496805555558</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added business and system exception handling with email notifications
</commit_message>
<xml_diff>
--- a/Data/Output/PartnershipEmails_Report.xlsx
+++ b/Data/Output/PartnershipEmails_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{65BF24DD-A887-4BEA-97D7-2185F6644BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD83C03-83BF-49DF-90CE-95B10A50FA28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC0EF0-F950-48BD-96D2-A50692F5D882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partnership_Emails" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="14">
   <si>
     <t>Date Processed</t>
   </si>
@@ -133,10 +133,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -764,6 +760,167 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45855.999027777776</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45856.032638888886</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45856.059907407405</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45856.071342592593</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45856.097303240742</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45856.104791666665</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45856.108865740738</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initialize filtered list collections
</commit_message>
<xml_diff>
--- a/Data/Output/PartnershipEmails_Report.xlsx
+++ b/Data/Output/PartnershipEmails_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC0EF0-F950-48BD-96D2-A50692F5D882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88408C1-475F-435D-BB56-5C3F4C53AA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partnership_Emails" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="14">
   <si>
     <t>Date Processed</t>
   </si>
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -921,6 +921,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45857.00277777778</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored based on Analyze Project results: removed unused dependencies, fixed warnings, and optimized workflows.
</commit_message>
<xml_diff>
--- a/Data/Output/PartnershipEmails_Report.xlsx
+++ b/Data/Output/PartnershipEmails_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C8579B-4A8E-4672-983D-F11231AAA110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{72C8579B-4A8E-4672-983D-F11231AAA110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25A99DE8-DD99-4798-AF0B-5D6CE07B6049}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="20">
   <si>
     <t>Date Processed</t>
   </si>
@@ -42,9 +42,6 @@
     <t>VAT ID</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Email Subject</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Bahnhofstrasse 45, Munich, Germany_x000D_</t>
+  </si>
+  <si>
+    <t>Email Address</t>
   </si>
 </sst>
 </file>
@@ -128,10 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +447,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -457,22 +458,22 @@
         <v>45857.941134259258</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -480,22 +481,22 @@
         <v>45857.972418981481</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -503,19 +504,19 @@
         <v>45857.972418981481</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -523,19 +524,19 @@
         <v>45857.972418981481</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -543,22 +544,22 @@
         <v>45857.999456018515</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -566,22 +567,22 @@
         <v>45857.999456018515</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,22 +590,160 @@
         <v>45857.999456018515</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45859.800729166665</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45859.800729166665</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45859.800729166665</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45859.80741898148</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45859.80741898148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45859.80741898148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>